<commit_message>
Pflichtanlagen Vorbereitung ohne Berechnung
</commit_message>
<xml_diff>
--- a/hhdaten/bewegungsdaten.xlsx
+++ b/hhdaten/bewegungsdaten.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11010" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11010"/>
   </bookViews>
   <sheets>
     <sheet name="Planung" sheetId="1" r:id="rId1"/>
@@ -6698,7 +6698,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6708,13 +6708,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1116"/>
   <sheetViews>
-    <sheetView topLeftCell="B271" workbookViewId="0">
-      <selection activeCell="A1117" sqref="A1117:XFD1117"/>
+    <sheetView tabSelected="1" topLeftCell="C1063" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+    <col min="5" max="5" width="61.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -75371,7 +75371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:J109"/>
     </sheetView>
   </sheetViews>

</xml_diff>